<commit_message>
Updated license and reformatted all .rb and .R files using rubymine editor
</commit_message>
<xml_diff>
--- a/Install/Parameter UQ Repository V1.0.xlsx
+++ b/Install/Parameter UQ Repository V1.0.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="13740"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="97">
   <si>
     <t>Category</t>
   </si>
@@ -172,9 +172,6 @@
     <t>FlowPerExteriorArea</t>
   </si>
   <si>
-    <t>Lights</t>
-  </si>
-  <si>
     <t>WattsPerSpaceFloorArea</t>
   </si>
   <si>
@@ -308,12 +305,18 @@
   </si>
   <si>
     <t>ThermostatSetpointCooling</t>
+  </si>
+  <si>
+    <t>WattsPerSpaceFloorAreax</t>
+  </si>
+  <si>
+    <t>Lightsxxx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -658,77 +661,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -742,7 +680,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -777,7 +715,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -812,7 +750,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1024,8 +962,8 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
+      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1075,7 +1013,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>9</v>
@@ -1230,7 +1168,7 @@
         <v>47</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" s="46" t="s">
         <v>44</v>
@@ -1284,7 +1222,7 @@
         <v>48</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D10" s="46" t="s">
         <v>44</v>
@@ -1311,7 +1249,7 @@
         <v>48</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D11" s="46" t="s">
         <v>44</v>
@@ -1338,7 +1276,7 @@
         <v>48</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D12" s="46" t="s">
         <v>44</v>
@@ -1365,7 +1303,7 @@
         <v>48</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D13" s="46" t="s">
         <v>44</v>
@@ -1392,7 +1330,7 @@
         <v>48</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D14" s="46" t="s">
         <v>44</v>
@@ -1419,7 +1357,7 @@
         <v>48</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D15" s="46" t="s">
         <v>44</v>
@@ -1446,7 +1384,7 @@
         <v>48</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D16" s="46" t="s">
         <v>44</v>
@@ -1473,7 +1411,7 @@
         <v>48</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D17" s="46" t="s">
         <v>44</v>
@@ -1500,7 +1438,7 @@
         <v>48</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D18" s="46" t="s">
         <v>44</v>
@@ -1527,7 +1465,7 @@
         <v>48</v>
       </c>
       <c r="C19" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D19" s="46" t="s">
         <v>44</v>
@@ -1554,7 +1492,7 @@
         <v>48</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D20" s="46" t="s">
         <v>44</v>
@@ -1602,13 +1540,13 @@
     </row>
     <row r="22" spans="1:9" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>51</v>
+        <v>95</v>
       </c>
       <c r="D22" s="24" t="s">
         <v>43</v>
@@ -1632,10 +1570,10 @@
     <row r="23" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="58"/>
       <c r="B23" s="36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D23" s="36" t="s">
         <v>43</v>
@@ -1659,10 +1597,10 @@
     <row r="24" spans="1:9" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="59"/>
       <c r="B24" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>44</v>
@@ -1685,13 +1623,13 @@
     </row>
     <row r="25" spans="1:9" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A25" s="50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="30" t="s">
         <v>57</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>58</v>
       </c>
       <c r="D25" s="36" t="s">
         <v>44</v>
@@ -1715,10 +1653,10 @@
     <row r="26" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="50"/>
       <c r="B26" s="36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D26" s="36" t="s">
         <v>44</v>
@@ -1742,10 +1680,10 @@
     <row r="27" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="50"/>
       <c r="B27" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D27" s="36" t="s">
         <v>44</v>
@@ -1769,10 +1707,10 @@
     <row r="28" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="50"/>
       <c r="B28" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D28" s="36" t="s">
         <v>44</v>
@@ -1796,10 +1734,10 @@
     <row r="29" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="50"/>
       <c r="B29" s="36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D29" s="36" t="s">
         <v>44</v>
@@ -1823,10 +1761,10 @@
     <row r="30" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="50"/>
       <c r="B30" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="32" t="s">
         <v>62</v>
-      </c>
-      <c r="C30" s="32" t="s">
-        <v>63</v>
       </c>
       <c r="D30" s="36" t="s">
         <v>44</v>
@@ -1850,10 +1788,10 @@
     <row r="31" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="50"/>
       <c r="B31" s="36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C31" s="32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D31" s="36" t="s">
         <v>44</v>
@@ -1877,10 +1815,10 @@
     <row r="32" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="50"/>
       <c r="B32" s="36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D32" s="36" t="s">
         <v>44</v>
@@ -1904,10 +1842,10 @@
     <row r="33" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="50"/>
       <c r="B33" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C33" s="38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D33" s="36" t="s">
         <v>44</v>
@@ -1931,10 +1869,10 @@
     <row r="34" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="50"/>
       <c r="B34" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C34" s="38" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D34" s="36" t="s">
         <v>44</v>
@@ -1958,10 +1896,10 @@
     <row r="35" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="50"/>
       <c r="B35" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C35" s="38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D35" s="36" t="s">
         <v>44</v>
@@ -1985,10 +1923,10 @@
     <row r="36" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="50"/>
       <c r="B36" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="38" t="s">
         <v>69</v>
-      </c>
-      <c r="C36" s="38" t="s">
-        <v>70</v>
       </c>
       <c r="D36" s="36" t="s">
         <v>44</v>
@@ -2012,10 +1950,10 @@
     <row r="37" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="50"/>
       <c r="B37" s="36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C37" s="38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D37" s="36" t="s">
         <v>44</v>
@@ -2039,10 +1977,10 @@
     <row r="38" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="50"/>
       <c r="B38" s="36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C38" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D38" s="36" t="s">
         <v>44</v>
@@ -2066,10 +2004,10 @@
     <row r="39" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="50"/>
       <c r="B39" s="36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C39" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D39" s="36" t="s">
         <v>44</v>
@@ -2093,10 +2031,10 @@
     <row r="40" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="50"/>
       <c r="B40" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="38" t="s">
         <v>74</v>
-      </c>
-      <c r="C40" s="38" t="s">
-        <v>75</v>
       </c>
       <c r="D40" s="36" t="s">
         <v>44</v>
@@ -2120,10 +2058,10 @@
     <row r="41" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="50"/>
       <c r="B41" s="46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C41" s="43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D41" s="46" t="s">
         <v>44</v>
@@ -2147,10 +2085,10 @@
     <row r="42" spans="1:9" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="51"/>
       <c r="B42" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="42" t="s">
         <v>77</v>
-      </c>
-      <c r="C42" s="42" t="s">
-        <v>78</v>
       </c>
       <c r="D42" s="19" t="s">
         <v>44</v>
@@ -2173,13 +2111,13 @@
     </row>
     <row r="43" spans="1:9" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="B43" s="47" t="s">
+      <c r="C43" s="47" t="s">
         <v>93</v>
-      </c>
-      <c r="C43" s="47" t="s">
-        <v>94</v>
       </c>
       <c r="D43" s="46" t="s">
         <v>44</v>
@@ -2203,10 +2141,10 @@
     <row r="44" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="31"/>
       <c r="B44" s="48" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C44" s="48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D44" s="46" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
Updates for Openstudio 1.1.14
Updated gem installs and testinstall scripts
Updated test.osm to a new and smaller files that runs faster.  Still
need to update utility bills to be consistent
</commit_message>
<xml_diff>
--- a/Install/Parameter UQ Repository V1.0.xlsx
+++ b/Install/Parameter UQ Repository V1.0.xlsx
@@ -962,8 +962,8 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1549,7 +1549,7 @@
         <v>95</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E22" s="26" t="s">
         <v>10</v>
@@ -1982,8 +1982,8 @@
       <c r="C38" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="D38" s="36" t="s">
-        <v>44</v>
+      <c r="D38" s="46" t="s">
+        <v>43</v>
       </c>
       <c r="E38" s="33" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Trying to debug the problems with extracting meters
trying different building models to try to debug the problems with
facility meters (gas and electric whole building)
</commit_message>
<xml_diff>
--- a/Install/Parameter UQ Repository V1.0.xlsx
+++ b/Install/Parameter UQ Repository V1.0.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="13740"/>
@@ -15,7 +15,7 @@
     <definedName name="_ENREF_5" localSheetId="2">References!$A$11</definedName>
     <definedName name="_ENREF_6" localSheetId="2">References!$A$12</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -313,7 +313,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -658,77 +658,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -742,7 +677,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -777,7 +712,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -810,9 +745,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -845,6 +797,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1024,8 +993,8 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
+      <pane ySplit="2" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1098,7 +1067,7 @@
         <v>37</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>10</v>
@@ -1152,7 +1121,7 @@
         <v>39</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>10</v>
@@ -1638,7 +1607,7 @@
         <v>51</v>
       </c>
       <c r="D23" s="36" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E23" s="33" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Code Cleanup, error printing, and verbose options
Cleaned up some code, added more error printing to
Uncertainty_parameters, fixed gui stuff in run_all_osms
</commit_message>
<xml_diff>
--- a/Install/Parameter UQ Repository V1.0.xlsx
+++ b/Install/Parameter UQ Repository V1.0.xlsx
@@ -310,7 +310,7 @@
     <t>WattsPerSpaceFloorAreax</t>
   </si>
   <si>
-    <t>Lightsxxx</t>
+    <t>Lights</t>
   </si>
 </sst>
 </file>
@@ -962,8 +962,8 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1036,7 +1036,7 @@
         <v>37</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Revert "Merge pull request #5 from Argonne-National-Laboratory/debug-compute-sensitivity-code"
This reverts commit 6f2953f5397c9b30c66bb8813dc4598a14f101b8, reversing
changes made to e94b9ed9a881f26ef7fe78198ad306189eb9a5c7.
</commit_message>
<xml_diff>
--- a/Install/Parameter UQ Repository V1.0.xlsx
+++ b/Install/Parameter UQ Repository V1.0.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="13740"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="97">
   <si>
     <t>Category</t>
   </si>
@@ -307,7 +307,10 @@
     <t>ThermostatSetpointCooling</t>
   </si>
   <si>
-    <t>Lights</t>
+    <t>WattsPerSpaceFloorAreax</t>
+  </si>
+  <si>
+    <t>Lightsxxx</t>
   </si>
 </sst>
 </file>
@@ -745,23 +748,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -797,23 +783,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -993,8 +962,8 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1036,7 @@
         <v>37</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>10</v>
@@ -1093,7 +1062,7 @@
       <c r="C4" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="15" t="s">
         <v>44</v>
       </c>
       <c r="E4" s="5" t="s">
@@ -1120,7 +1089,7 @@
       <c r="C5" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="15" t="s">
         <v>44</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -1147,7 +1116,7 @@
       <c r="C6" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" s="15" t="s">
         <v>44</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -1174,7 +1143,7 @@
       <c r="C7" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="15" t="s">
         <v>44</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -1228,7 +1197,7 @@
       <c r="C9" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="15" t="s">
         <v>44</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -1552,7 +1521,7 @@
       <c r="C21" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="46" t="s">
+      <c r="D21" s="19" t="s">
         <v>44</v>
       </c>
       <c r="E21" s="20" t="s">
@@ -1574,12 +1543,12 @@
         <v>52</v>
       </c>
       <c r="B22" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="C22" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="46" t="s">
+      <c r="D22" s="24" t="s">
         <v>43</v>
       </c>
       <c r="E22" s="26" t="s">
@@ -1606,8 +1575,8 @@
       <c r="C23" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="46" t="s">
-        <v>44</v>
+      <c r="D23" s="36" t="s">
+        <v>43</v>
       </c>
       <c r="E23" s="33" t="s">
         <v>10</v>
@@ -1633,7 +1602,7 @@
       <c r="C24" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="46" t="s">
+      <c r="D24" s="19" t="s">
         <v>44</v>
       </c>
       <c r="E24" s="20" t="s">
@@ -1662,7 +1631,7 @@
       <c r="C25" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="D25" s="46" t="s">
+      <c r="D25" s="36" t="s">
         <v>44</v>
       </c>
       <c r="E25" s="33" t="s">
@@ -1689,7 +1658,7 @@
       <c r="C26" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="46" t="s">
+      <c r="D26" s="36" t="s">
         <v>44</v>
       </c>
       <c r="E26" s="33" t="s">
@@ -1716,7 +1685,7 @@
       <c r="C27" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="46" t="s">
+      <c r="D27" s="36" t="s">
         <v>44</v>
       </c>
       <c r="E27" s="33" t="s">
@@ -1743,7 +1712,7 @@
       <c r="C28" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="D28" s="46" t="s">
+      <c r="D28" s="36" t="s">
         <v>44</v>
       </c>
       <c r="E28" s="33" t="s">
@@ -1770,7 +1739,7 @@
       <c r="C29" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="D29" s="46" t="s">
+      <c r="D29" s="36" t="s">
         <v>44</v>
       </c>
       <c r="E29" s="33" t="s">
@@ -1797,7 +1766,7 @@
       <c r="C30" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="D30" s="46" t="s">
+      <c r="D30" s="36" t="s">
         <v>44</v>
       </c>
       <c r="E30" s="33" t="s">
@@ -1824,7 +1793,7 @@
       <c r="C31" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="46" t="s">
+      <c r="D31" s="36" t="s">
         <v>44</v>
       </c>
       <c r="E31" s="33" t="s">
@@ -1851,7 +1820,7 @@
       <c r="C32" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="46" t="s">
+      <c r="D32" s="36" t="s">
         <v>44</v>
       </c>
       <c r="E32" s="33" t="s">
@@ -1878,7 +1847,7 @@
       <c r="C33" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="D33" s="46" t="s">
+      <c r="D33" s="36" t="s">
         <v>44</v>
       </c>
       <c r="E33" s="33" t="s">
@@ -1905,7 +1874,7 @@
       <c r="C34" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="D34" s="46" t="s">
+      <c r="D34" s="36" t="s">
         <v>44</v>
       </c>
       <c r="E34" s="33" t="s">
@@ -1932,7 +1901,7 @@
       <c r="C35" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="D35" s="46" t="s">
+      <c r="D35" s="36" t="s">
         <v>44</v>
       </c>
       <c r="E35" s="33" t="s">
@@ -1959,7 +1928,7 @@
       <c r="C36" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="D36" s="46" t="s">
+      <c r="D36" s="36" t="s">
         <v>44</v>
       </c>
       <c r="E36" s="33" t="s">
@@ -1986,7 +1955,7 @@
       <c r="C37" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="46" t="s">
+      <c r="D37" s="36" t="s">
         <v>44</v>
       </c>
       <c r="E37" s="33" t="s">
@@ -2013,7 +1982,7 @@
       <c r="C38" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="D38" s="46" t="s">
+      <c r="D38" s="36" t="s">
         <v>44</v>
       </c>
       <c r="E38" s="33" t="s">
@@ -2040,7 +2009,7 @@
       <c r="C39" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="D39" s="46" t="s">
+      <c r="D39" s="36" t="s">
         <v>44</v>
       </c>
       <c r="E39" s="33" t="s">
@@ -2067,7 +2036,7 @@
       <c r="C40" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="D40" s="46" t="s">
+      <c r="D40" s="36" t="s">
         <v>44</v>
       </c>
       <c r="E40" s="33" t="s">
@@ -2121,7 +2090,7 @@
       <c r="C42" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="D42" s="46" t="s">
+      <c r="D42" s="19" t="s">
         <v>44</v>
       </c>
       <c r="E42" s="20" t="s">

</xml_diff>